<commit_message>
fixed GET id bug
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Duke\2_2020_Spring\ECE_568\erss-hwk2-zq29-jx95\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05A2BE1-84A7-4EA3-B94D-9D3C97829B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE7ECD-063C-4B0F-9131-99107BB91D0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
add one test case
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Duke\2_2020_Spring\ECE_568\erss-hwk2-zq29-jx95\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE7ECD-063C-4B0F-9131-99107BB91D0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEDC134-A670-41B5-A3E9-5A96EC7F573B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>No</t>
+    <t>If you want to check our automatic test, do not run docker as a daemon since we're printing test information to stdout</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -513,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -671,7 +671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>